<commit_message>
V2 generation successfully imported.
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -3,32 +3,128 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95417F5C-4A4F-46B0-9E4E-CA9800FEF060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A94D53B-9E66-4EDA-8D93-670E8A1AB1E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="0" windowWidth="11420" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5510" yWindow="0" windowWidth="18150" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Facilities" sheetId="1" r:id="rId1"/>
     <sheet name="Facilities schedule" sheetId="2" r:id="rId2"/>
     <sheet name="Devices" sheetId="3" r:id="rId3"/>
-    <sheet name="DropDownData" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Global settings" sheetId="5" r:id="rId4"/>
+    <sheet name="DropDownData" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+  <si>
+    <t>Facility ID</t>
+  </si>
+  <si>
+    <t>Facility name</t>
+  </si>
+  <si>
+    <t>Facility city</t>
+  </si>
+  <si>
+    <t>Facility state</t>
+  </si>
+  <si>
+    <t>IANA zone ID</t>
+  </si>
+  <si>
+    <t>Facility Active=1/Inactive=0</t>
+  </si>
+  <si>
+    <t>Operating hours Dlog throttle speed
+(KBps)</t>
+  </si>
+  <si>
+    <t>Non-operating hours Dlog throttle speed (KBps)</t>
+  </si>
+  <si>
+    <t>Day of week</t>
+  </si>
+  <si>
+    <t>Data transmission start (24 Hour Clock)</t>
+  </si>
+  <si>
+    <t>Duration (Hours)</t>
+  </si>
+  <si>
+    <t>Device name</t>
+  </si>
+  <si>
+    <t>Serial number</t>
+  </si>
   <si>
     <t>Device Active=1/Inactive=0</t>
   </si>
   <si>
-    <t>Facility Active=1/Inactive=0</t>
+    <t>Global setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Dlog_URL</t>
+  </si>
+  <si>
+    <t>Dlog_API key</t>
+  </si>
+  <si>
+    <t>Dlog_Look back (days)</t>
+  </si>
+  <si>
+    <t>Dlog_Max per sync (dlogs)</t>
+  </si>
+  <si>
+    <t>Dlog_Collection enabled</t>
+  </si>
+  <si>
+    <t>America/Adak</t>
+  </si>
+  <si>
+    <t>America/Anchorage</t>
+  </si>
+  <si>
+    <t>America/Atka</t>
   </si>
   <si>
     <t>America/Boise</t>
   </si>
   <si>
+    <t>America/Chicago</t>
+  </si>
+  <si>
+    <t>America/Denver</t>
+  </si>
+  <si>
+    <t>America/Detroit</t>
+  </si>
+  <si>
+    <t>America/Fort_Wayne</t>
+  </si>
+  <si>
+    <t>America/Indiana/Indianapolis</t>
+  </si>
+  <si>
+    <t>America/Indiana/Knox</t>
+  </si>
+  <si>
     <t>America/Indiana/Marengo</t>
   </si>
   <si>
@@ -47,18 +143,36 @@
     <t>America/Indiana/Winamac</t>
   </si>
   <si>
+    <t>America/Indianapolis</t>
+  </si>
+  <si>
     <t>America/Juneau</t>
   </si>
   <si>
+    <t>America/Kentucky/Louisville</t>
+  </si>
+  <si>
     <t>America/Kentucky/Monticello</t>
   </si>
   <si>
+    <t>America/Knox_IN</t>
+  </si>
+  <si>
+    <t>America/Los_Angeles</t>
+  </si>
+  <si>
+    <t>America/Louisville</t>
+  </si>
+  <si>
     <t>America/Menominee</t>
   </si>
   <si>
     <t>America/Metlakatla</t>
   </si>
   <si>
+    <t>America/New_York</t>
+  </si>
+  <si>
     <t>America/Nome</t>
   </si>
   <si>
@@ -71,136 +185,61 @@
     <t>America/North_Dakota/New_Salem</t>
   </si>
   <si>
+    <t>America/Phoenix</t>
+  </si>
+  <si>
+    <t>America/Shiprock</t>
+  </si>
+  <si>
     <t>America/Sitka</t>
   </si>
   <si>
     <t>America/Yakutat</t>
   </si>
   <si>
-    <t>America/Adak</t>
-  </si>
-  <si>
-    <t>America/Atka</t>
+    <t>Navajo</t>
+  </si>
+  <si>
+    <t>Pacific/Honolulu</t>
+  </si>
+  <si>
+    <t>Pacific/Johnston</t>
+  </si>
+  <si>
+    <t>US/Alaska</t>
   </si>
   <si>
     <t>US/Aleutian</t>
   </si>
   <si>
-    <t>America/Anchorage</t>
-  </si>
-  <si>
-    <t>US/Alaska</t>
-  </si>
-  <si>
-    <t>America/Chicago</t>
+    <t>US/Arizona</t>
   </si>
   <si>
     <t>US/Central</t>
   </si>
   <si>
-    <t>America/Denver</t>
-  </si>
-  <si>
-    <t>America/Shiprock</t>
-  </si>
-  <si>
-    <t>Navajo</t>
+    <t>US/Eastern</t>
+  </si>
+  <si>
+    <t>US/East-Indiana</t>
+  </si>
+  <si>
+    <t>US/Hawaii</t>
+  </si>
+  <si>
+    <t>US/Indiana-Starke</t>
+  </si>
+  <si>
+    <t>US/Michigan</t>
   </si>
   <si>
     <t>US/Mountain</t>
   </si>
   <si>
-    <t>America/Detroit</t>
-  </si>
-  <si>
-    <t>US/Michigan</t>
-  </si>
-  <si>
-    <t>America/Indiana/Indianapolis</t>
-  </si>
-  <si>
-    <t>America/Fort_Wayne</t>
-  </si>
-  <si>
-    <t>America/Indianapolis</t>
-  </si>
-  <si>
-    <t>US/East-Indiana</t>
-  </si>
-  <si>
-    <t>America/Indiana/Knox</t>
-  </si>
-  <si>
-    <t>America/Knox_IN</t>
-  </si>
-  <si>
-    <t>US/Indiana-Starke</t>
-  </si>
-  <si>
-    <t>America/Kentucky/Louisville</t>
-  </si>
-  <si>
-    <t>America/Louisville</t>
-  </si>
-  <si>
-    <t>America/Los_Angeles</t>
-  </si>
-  <si>
-    <t>America/New_York</t>
-  </si>
-  <si>
-    <t>US/Eastern</t>
-  </si>
-  <si>
-    <t>America/Phoenix</t>
-  </si>
-  <si>
-    <t>US/Arizona</t>
-  </si>
-  <si>
-    <t>Pacific/Honolulu</t>
-  </si>
-  <si>
-    <t>Pacific/Johnston</t>
-  </si>
-  <si>
-    <t>US/Hawaii</t>
-  </si>
-  <si>
     <t>US/Pacific</t>
   </si>
   <si>
     <t>US/Pacific-New</t>
-  </si>
-  <si>
-    <t>Duration (Hours)</t>
-  </si>
-  <si>
-    <t>Facility ID</t>
-  </si>
-  <si>
-    <t>Device name</t>
-  </si>
-  <si>
-    <t>Serial number</t>
-  </si>
-  <si>
-    <t>Facility name</t>
-  </si>
-  <si>
-    <t>Facility city</t>
-  </si>
-  <si>
-    <t>Facility state</t>
-  </si>
-  <si>
-    <t>IANA zone ID</t>
-  </si>
-  <si>
-    <t>Day of week</t>
-  </si>
-  <si>
-    <t>Data transmission start (24 Hour Clock)</t>
   </si>
 </sst>
 </file>
@@ -210,7 +249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +261,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,10 +291,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -260,11 +308,24 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -284,7 +345,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -304,6 +365,61 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7343775" y="885825"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A66565C-C95A-41E2-9BC5-A9C687E6BA3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11645900" y="184150"/>
           <a:ext cx="184731" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -661,11 +777,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,33 +792,41 @@
     <col min="4" max="4" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.54296875" style="2" customWidth="1"/>
     <col min="6" max="6" width="25.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="7" max="7" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9yjTa+ObFIPppufl5Wpx31cx01EXYQJPlo+StThR+WVMm9Eph7vzyLYiHyyaevwUcVDaeAMh32Q/9Bq5g3VJwg==" saltValue="kcimRzSVGYwj607JKJ0f4g==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="cEUx4CN0TuZIPE/TLU+Ryi4I3uSH5XW2GaG+IxUM/jE6Q88QUEKjKQSg9+cwVTsfoyIQkAcRW2HgV9cpFhIXUw==" saltValue="LaJHCDSt5LRbOCBMDzTWRw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate function="countNums"/>
-  <dataValidations count="9">
+  <dataValidations count="10">
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters._x000a_Special characters are not allowed._x000a_Duplicate Facility ID is not allowed." sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Facility Active=1/Inactive=0" error="Value must be 0 and 1." sqref="F1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="IANA zone ID" error="Select a valid IANA zone ID from the dropdown." sqref="E1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
@@ -710,17 +834,20 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="Facility city" error="Facility city accepts only alphabetic characters." sqref="C1" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>AND(ISTEXT(C1),ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(C1,ROW(INDIRECT("1:"&amp;LEN(C1))),1),"abcdefghijklmnopqrstuvwxyz ABCDEFGHIJKLMNOPQRSTUVWXYZ"))))</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="Facility name" error="Duplicate facility name is not allowed." sqref="B1" xr:uid="{00000000-0002-0000-0000-000005000000}">
+      <formula1>COUNTIF($B:$B,B1)=1</formula1>
+    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility name" error="Duplicate facility name is not allowed." sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>COUNTIF($B:$B,B2)=1</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="Facility name" error="Duplicate facility name is not allowed." sqref="B1" xr:uid="{00000000-0002-0000-0000-000005000000}">
-      <formula1>COUNTIF($B:$B,B1)=1</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters._x000a_Duplicate facility ID is not allowed." sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>AND(LEN(A2)&lt;=20,COUNTIF($A:$A,A2)=1)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility state" error="Facility state requires alphanumeric characters between 2 and 3." sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>AND(ISTEXT(D2),LEN(D2)&gt;=2,LEN(D2)&lt;=3,ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(D2,ROW(INDIRECT("1:"&amp;LEN(D2))),1),"abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789"))))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility state" error="Facility state requires alphanumeric characters between 2 to 3." sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
+      <formula1>AND(LEN(D2)&gt;=2,LEN(D2)&lt;=3,ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(D2,ROW(INDIRECT("1:"&amp;LEN(D2))),1),"abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ0123456789"))))</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dlog throttle speed (KBps)" error="Value must be greater than or equal to 0." sqref="G1:G1048576 H1:H1048576" xr:uid="{00000000-0002-0000-0000-000009000000}">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -728,19 +855,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility Active=1/Inactive=0" error="Value must be 0 or 1." xr:uid="{00000000-0002-0000-0000-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility Active=1/Inactive=0" error="Value must be 0 or 1." xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>DropDownData!$C$1:$C$2</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IANA zone ID" error="Select a valid IANA zone ID from the dropdown." xr:uid="{00000000-0002-0000-0000-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IANA zone ID" error="Select a valid IANA zone ID from the dropdown." xr:uid="{00000000-0002-0000-0000-00000B000000}">
           <x14:formula1>
             <xm:f>DropDownData!$A$1:$A$49</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility city" error="Facility city accepts only alphabetic and special characters." xr:uid="{00000000-0002-0000-0000-00000B000000}">
+        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility city" error="Facility city accepts only alphabetic and special characters." xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>AND(SUMPRODUCT(--ISNUMBER(SEARCH(DropDownData!$E$1:$E$10,C2)))=0)</xm:f>
           </x14:formula1>
@@ -754,7 +881,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -766,44 +893,85 @@
     <col min="1" max="1" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.453125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="4" max="4" width="16.81640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Za36l1vuYffeWKwu0ERAkydPYn6eolRLttN1fbU1NgHBzGZlG1kQOwMsIwLsK1sQscTX69kOaOuWcWhz2Y9a2Q==" saltValue="ciqzZ29IRLkfMKhFpPWQSQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
-  <dataValidations count="6">
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="7">
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Day of week" error="Day of week accepts only number between 1 to 7._x000a_" sqref="B1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters._x000a_Special characters are not allowed." sqref="A1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters." sqref="A16:A1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <formula1>AND(LEN(A16)&lt;=20)</formula1>
+    </dataValidation>
     <dataValidation type="time" allowBlank="1" showInputMessage="1" errorTitle="Data transmission start" error="Data transmission start must be in HH:MM format._x000a_Data Transmission start only accepts value between 00:00 to 23:59." sqref="C1" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters." sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>AND(LEN(A2)&lt;=20,COUNTIF($A:$A,A2)=1)</formula1>
-    </dataValidation>
     <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Data transmission start" error="Data transmission start must be in HH:MM format._x000a_Data transmission start only accepts value between 00:00 to 23:59." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters._x000a_Special characters are not allowed." sqref="A2:A15" xr:uid="{22582600-DBC3-4F36-ACC7-8480B18BD177}">
+      <formula1>AND(ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(A2,ROW(INDIRECT("1:"&amp;LEN(A2))),1),"0123456789 abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ"))),LEN(A2)&lt;=20)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -816,13 +984,13 @@
           <x14:formula1>
             <xm:f>DropDownData!$D$1:$D$97</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D16:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Day of week" error="Day of week accepts only number between 1 to 7._x000a_" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>DropDownData!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>B16:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -834,15 +1002,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD51"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="2"/>
@@ -850,34 +1018,34 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yIzVix5t9EnAlftsTvYz0VWXhMW7z4E32kpZ1LXjqxdgxd6kLBEjDqPOssUwDnlHwhtAv0t0/9RAcQT0oTuXYA==" saltValue="rKbruwzMCAdu/hOlhnks8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Qf08DjJWLeX35R9PhZLFSFMboaJMqZhBnPoblCKYYWNkw5pVfeukcxG3bfEgi0YPYOX/C6lryy/sr2ZwGy9gTA==" saltValue="6KTz/5XBhBbGSGWPfUNM1w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="7">
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Device Active=1/Inactive=0" error="Value must be 0 or 1." sqref="D1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" errorTitle="Device name" error="Device name length must be less than or equal to 20 characters.._x000a_Special characters are not allowed._x000a_Duplicate device name is not allowed._x000a_" sqref="A1" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters._x000a_Special characters are not allowed." sqref="C1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Device name" error="Device name length must be less than or equal to 20 characters._x000a_Special characters are not allowed._x000a_Duplicate device name is not allowed._x000a_" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>AND(ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(A2,ROW(INDIRECT("1:"&amp;LEN(A2))),1),"0123456789 abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ"))),LEN(A2)&lt;=20,COUNTIF($A:$A,A2)=1)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Facility ID" error="Facility ID length must be less than or equal to 20 characters." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0200-000004000000}">
-      <formula1>AND(LEN(C2)&lt;=20,COUNTIF($C:$C,C2)=1)</formula1>
+      <formula1>AND(LEN(C2)&lt;=20)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Serial number" error="Serial number length must be 7 characters._x000a_Special characters are not allowed._x000a_Duplicate serial number is not allowed." sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>AND(ISNUMBER(SUMPRODUCT(SEARCH("~"&amp;MID(B2,ROW(INDIRECT("1:"&amp;LEN(B2))),1),"0123456789 abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ"))),LEN(B2)=7,COUNTIF($B:$B,B2)=1)</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -898,6 +1066,82 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Q+bVPWI8X9f5leHmuJhDft4CsZS9Bv4OylGyWKQJ/M+7Ei5coYBpo5BpoD8UsICgFuR3L4nADm2jBFa6ZCOfqg==" saltValue="Qv+2HDLKOzREjj2GvvS/rw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="3">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Dlog_Collection enabled" error="Value must be TRUE or FALSE." sqref="B6" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dlog_Max per sync (dlogs)" error="Value must be numeric and greater than 0." sqref="B5" xr:uid="{00000000-0002-0000-0300-000001000000}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Dlog_Look back (days)" error="Value must be between 1 to 1440." sqref="B4" xr:uid="{00000000-0002-0000-0300-000002000000}">
+      <formula1>1</formula1>
+      <formula2>1440</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -913,7 +1157,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -947,7 +1191,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -961,7 +1205,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -975,7 +1219,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -1003,7 +1247,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1017,7 +1261,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>1.75</v>
@@ -1028,7 +1272,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1039,7 +1283,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>2.25</v>
@@ -1050,7 +1294,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>2.5</v>
@@ -1058,7 +1302,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>2.75</v>
@@ -1066,7 +1310,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1074,7 +1318,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>3.25</v>
@@ -1082,7 +1326,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D15">
         <v>3.5</v>
@@ -1090,7 +1334,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>3.75</v>
@@ -1098,7 +1342,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -1106,7 +1350,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>4.25</v>
@@ -1122,7 +1366,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>4.75</v>
@@ -1130,7 +1374,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1138,7 +1382,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22">
         <v>5.25</v>
@@ -1146,7 +1390,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>5.5</v>
@@ -1154,7 +1398,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D24">
         <v>5.75</v>
@@ -1162,7 +1406,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D25">
         <v>6</v>
@@ -1170,7 +1414,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>6.25</v>
@@ -1178,7 +1422,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D27">
         <v>6.5</v>
@@ -1186,7 +1430,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D28">
         <v>6.75</v>
@@ -1194,7 +1438,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -1202,7 +1446,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D30">
         <v>7.25</v>
@@ -1210,7 +1454,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D31">
         <v>7.5</v>
@@ -1218,7 +1462,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D32">
         <v>7.75</v>
@@ -1226,7 +1470,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D33">
         <v>8</v>
@@ -1234,7 +1478,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D34">
         <v>8.25</v>
@@ -1242,7 +1486,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D35">
         <v>8.5</v>
@@ -1250,7 +1494,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D36">
         <v>8.75</v>
@@ -1258,7 +1502,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D37">
         <v>9</v>
@@ -1266,7 +1510,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D38">
         <v>9.25</v>
@@ -1274,7 +1518,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="D39">
         <v>9.5</v>
@@ -1282,7 +1526,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D40">
         <v>9.75</v>
@@ -1290,7 +1534,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -1298,7 +1542,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D42">
         <v>10.25</v>
@@ -1306,7 +1550,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="D43">
         <v>10.5</v>
@@ -1314,7 +1558,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D44">
         <v>10.75</v>
@@ -1322,7 +1566,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D45">
         <v>11</v>
@@ -1330,7 +1574,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D46">
         <v>11.25</v>
@@ -1338,7 +1582,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D47">
         <v>11.5</v>
@@ -1346,7 +1590,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D48">
         <v>11.75</v>
@@ -1354,7 +1598,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D49">
         <v>12</v>

</xml_diff>